<commit_message>
database integration tested, works
</commit_message>
<xml_diff>
--- a/src/materials.xlsx
+++ b/src/materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelle\Documents\Bytemaps - Clients\Catwee\Verzorgend Wassen LCA\lcatool\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE19AA-7183-4FAA-973F-8AD1AFEA6566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE84C477-02C7-4945-9246-EA331CF37BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Material name</t>
   </si>
   <si>
-    <t>Impact category UUID</t>
-  </si>
-  <si>
     <t>Impact category</t>
   </si>
   <si>
@@ -42,136 +39,88 @@
     <t>Result</t>
   </si>
   <si>
-    <t>419dc346-20f1-33cb-84f9-84fc0c19bff7</t>
-  </si>
-  <si>
     <t>Acidification</t>
   </si>
   <si>
     <t>molc H+ eq</t>
   </si>
   <si>
-    <t>1811fb08-9d8a-38b3-9880-cab2ff6d1462</t>
-  </si>
-  <si>
     <t>Climate change</t>
   </si>
   <si>
     <t>kg CO2 eq</t>
   </si>
   <si>
-    <t>98ef5107-1a84-34ae-88dc-0c84da5d2545</t>
-  </si>
-  <si>
     <t>Freshwater ecotoxicity</t>
   </si>
   <si>
     <t>CTUe</t>
   </si>
   <si>
-    <t>c8c7b326-58f6-37a3-a8d6-161575c3dfd0</t>
-  </si>
-  <si>
     <t>Freshwater eutrophication</t>
   </si>
   <si>
     <t>kg P eq</t>
   </si>
   <si>
-    <t>970632e5-0def-30ee-a6dd-a2a7026c0b7f</t>
-  </si>
-  <si>
     <t>Human toxicity, cancer effects</t>
   </si>
   <si>
     <t>CTUh</t>
   </si>
   <si>
-    <t>d597d9bd-f306-3ad3-af11-16e6dd0ac7ec</t>
-  </si>
-  <si>
     <t>Human toxicity, non-cancer effects</t>
   </si>
   <si>
-    <t>2d0a4c8e-3af2-344e-a4af-6191359bd649</t>
-  </si>
-  <si>
     <t>Ionizing radiation E (interim)</t>
   </si>
   <si>
-    <t>e2dedeec-7f64-31b5-b5c4-94e7553f45cc</t>
-  </si>
-  <si>
     <t>Ionizing radiation HH</t>
   </si>
   <si>
     <t>kBq U235 eq</t>
   </si>
   <si>
-    <t>1d5fb5db-5de3-3a87-9a8a-65ef0c905f5f</t>
-  </si>
-  <si>
     <t>Land use</t>
   </si>
   <si>
     <t>kg C deficit</t>
   </si>
   <si>
-    <t>7292c216-0cee-3a5f-96c3-cf389ee89db5</t>
-  </si>
-  <si>
     <t>Marine eutrophication</t>
   </si>
   <si>
     <t>kg N eq</t>
   </si>
   <si>
-    <t>9518b4ea-d7c1-3548-a4b6-977770f0954a</t>
-  </si>
-  <si>
     <t>Mineral, fossil &amp; ren resource depletion</t>
   </si>
   <si>
     <t>kg Sb eq</t>
   </si>
   <si>
-    <t>a18cef8f-5787-37ee-9498-53ec64aad901</t>
-  </si>
-  <si>
     <t>Ozone depletion</t>
   </si>
   <si>
     <t>kg CFC-11 eq</t>
   </si>
   <si>
-    <t>6827e043-b809-3a5c-825e-7ad31ce9c7bf</t>
-  </si>
-  <si>
     <t>Particulate matter</t>
   </si>
   <si>
     <t>kg PM2.5 eq</t>
   </si>
   <si>
-    <t>ced83ca3-af5a-38f0-8b59-bb7900894301</t>
-  </si>
-  <si>
     <t>Photochemical ozone formation</t>
   </si>
   <si>
     <t>kg NMVOC eq</t>
   </si>
   <si>
-    <t>9e3bd74a-7c72-3204-a5fc-7fea48270e89</t>
-  </si>
-  <si>
     <t>Terrestrial eutrophication</t>
   </si>
   <si>
     <t>molc N eq</t>
-  </si>
-  <si>
-    <t>0ce35b4d-0ee7-30fb-a3a5-32a94d223ded</t>
   </si>
   <si>
     <t>Water resource depletion</t>
@@ -496,252 +445,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>9.6602860000000006E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>2.2463347749999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D5">
         <v>0.18369574599999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>-5.0318100000000002E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1">
         <v>4.5270300000000002E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1">
         <v>3.6972900000000002E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>8.85865E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1">
         <v>5.1827699999999998E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>5.0227599999999996E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>42</v>
-      </c>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D16">
         <v>6.4636770000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D17">
         <v>1.32009E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>48</v>
-      </c>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D18">
         <v>6.8349000000000003E-4</v>

</xml_diff>